<commit_message>
13 OK, 14 started
</commit_message>
<xml_diff>
--- a/Curriculum.xlsx
+++ b/Curriculum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="23655" windowHeight="9705"/>
+    <workbookView xWindow="240" yWindow="312" windowWidth="23652" windowHeight="9708"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Практика: Черепаха</t>
   </si>
@@ -127,13 +127,43 @@
   </si>
   <si>
     <t>БИЛЕТЫ К ЗАЧЁТУ</t>
+  </si>
+  <si>
+    <t>2017 год</t>
+  </si>
+  <si>
+    <t>2016 год</t>
+  </si>
+  <si>
+    <t>2015 год</t>
+  </si>
+  <si>
+    <t>Тестирование программ</t>
+  </si>
+  <si>
+    <t>Арифметика с плавающей запятой</t>
+  </si>
+  <si>
+    <t>Проект «Обработка матриц»</t>
+  </si>
+  <si>
+    <t>Проект «Допиши игру Сапёр»</t>
+  </si>
+  <si>
+    <t>Разработка игры "Pacman"</t>
+  </si>
+  <si>
+    <t>Продолжение проекта Pacman</t>
+  </si>
+  <si>
+    <t>Сдача проекта Pacman</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +197,22 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -177,7 +223,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5F4EF"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,14 +241,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -505,236 +558,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D29"/>
+  <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="72.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="72.140625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="3.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="59.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="59.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="2" spans="2:6" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="F5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="F13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="F14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="F15" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="F16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="F17" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D24" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D25" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="3"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="F26" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="D30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab2.html"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab1.html"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab4.html"/>
-    <hyperlink ref="B6" r:id="rId4" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab5.html"/>
-    <hyperlink ref="B7" r:id="rId5" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab8.html"/>
-    <hyperlink ref="B8" r:id="rId6" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab10.html"/>
-    <hyperlink ref="B9" r:id="rId7" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab11.html"/>
-    <hyperlink ref="B10" r:id="rId8" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab13.html"/>
-    <hyperlink ref="B11" r:id="rId9" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab14.html"/>
-    <hyperlink ref="B12" r:id="rId10" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab17.html"/>
-    <hyperlink ref="B13" r:id="rId11" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab18.html"/>
-    <hyperlink ref="B14" r:id="rId12" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab19.html"/>
-    <hyperlink ref="B15" r:id="rId13" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab20.html"/>
-    <hyperlink ref="B16" r:id="rId14" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab21.html"/>
-    <hyperlink ref="B17" r:id="rId15" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab23.html"/>
-    <hyperlink ref="B18" r:id="rId16" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab25.html"/>
-    <hyperlink ref="B19" r:id="rId17" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab28.html"/>
-    <hyperlink ref="B20" r:id="rId18" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab29.html"/>
-    <hyperlink ref="B21" r:id="rId19" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab31.html"/>
-    <hyperlink ref="B29" r:id="rId20"/>
-    <hyperlink ref="D3" r:id="rId21" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab1.html"/>
-    <hyperlink ref="D4" r:id="rId22" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab2.html"/>
-    <hyperlink ref="D5" r:id="rId23" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab5.html"/>
-    <hyperlink ref="D6" r:id="rId24" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab6.html"/>
-    <hyperlink ref="D8" r:id="rId25" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab7.html"/>
-    <hyperlink ref="D13" r:id="rId26" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab9.html"/>
-    <hyperlink ref="D14" r:id="rId27" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab10.html"/>
-    <hyperlink ref="D15" r:id="rId28" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab11.html"/>
-    <hyperlink ref="D16" r:id="rId29" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab12.html"/>
-    <hyperlink ref="D12" r:id="rId30" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab15.html"/>
-    <hyperlink ref="D11" r:id="rId31" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab14.html"/>
-    <hyperlink ref="D17" r:id="rId32" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab16.html"/>
-    <hyperlink ref="D18" r:id="rId33" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab20.html"/>
-    <hyperlink ref="D19" r:id="rId34" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab22.html"/>
-    <hyperlink ref="D20" r:id="rId35" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab23.html"/>
-    <hyperlink ref="D21" r:id="rId36" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab25.html"/>
-    <hyperlink ref="D23" r:id="rId37" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab27.html"/>
-    <hyperlink ref="D24" r:id="rId38" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab28.html"/>
-    <hyperlink ref="D25" r:id="rId39" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab29.html"/>
+    <hyperlink ref="B5" r:id="rId1" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab2.html"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab1.html"/>
+    <hyperlink ref="B6" r:id="rId3" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab4.html"/>
+    <hyperlink ref="B7" r:id="rId4" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab5.html"/>
+    <hyperlink ref="B8" r:id="rId5" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab8.html"/>
+    <hyperlink ref="B9" r:id="rId6" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab10.html"/>
+    <hyperlink ref="B10" r:id="rId7" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab11.html"/>
+    <hyperlink ref="B11" r:id="rId8" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab13.html"/>
+    <hyperlink ref="B12" r:id="rId9" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab14.html"/>
+    <hyperlink ref="B13" r:id="rId10" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab17.html"/>
+    <hyperlink ref="B14" r:id="rId11" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab18.html"/>
+    <hyperlink ref="B15" r:id="rId12" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab19.html"/>
+    <hyperlink ref="B16" r:id="rId13" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab20.html"/>
+    <hyperlink ref="B17" r:id="rId14" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab21.html"/>
+    <hyperlink ref="B18" r:id="rId15" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab23.html"/>
+    <hyperlink ref="B19" r:id="rId16" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab25.html"/>
+    <hyperlink ref="B20" r:id="rId17" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab28.html"/>
+    <hyperlink ref="B21" r:id="rId18" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab29.html"/>
+    <hyperlink ref="B26" r:id="rId19" display="http://judge.mipt.ru/mipt_cs_on_python3/labs/lab31.html"/>
+    <hyperlink ref="B30" r:id="rId20"/>
+    <hyperlink ref="D4" r:id="rId21" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab1.html"/>
+    <hyperlink ref="D5" r:id="rId22" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab2.html"/>
+    <hyperlink ref="D6" r:id="rId23" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab5.html"/>
+    <hyperlink ref="D7" r:id="rId24" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab6.html"/>
+    <hyperlink ref="D9" r:id="rId25" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab7.html"/>
+    <hyperlink ref="D14" r:id="rId26" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab9.html"/>
+    <hyperlink ref="D15" r:id="rId27" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab10.html"/>
+    <hyperlink ref="D16" r:id="rId28" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab11.html"/>
+    <hyperlink ref="D17" r:id="rId29" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab12.html"/>
+    <hyperlink ref="D13" r:id="rId30" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab15.html"/>
+    <hyperlink ref="D12" r:id="rId31" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab14.html"/>
+    <hyperlink ref="D18" r:id="rId32" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab16.html"/>
+    <hyperlink ref="D19" r:id="rId33" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab20.html"/>
+    <hyperlink ref="D20" r:id="rId34" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab22.html"/>
+    <hyperlink ref="D21" r:id="rId35" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab23.html"/>
+    <hyperlink ref="D22" r:id="rId36" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab25.html"/>
+    <hyperlink ref="D24" r:id="rId37" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab27.html"/>
+    <hyperlink ref="D25" r:id="rId38" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab28.html"/>
+    <hyperlink ref="D26" r:id="rId39" display="http://judge.mipt.ru/mipt_cs_on_python3_2016/labs/lab29.html"/>
+    <hyperlink ref="B2" r:id="rId40"/>
+    <hyperlink ref="D2" r:id="rId41"/>
+    <hyperlink ref="F2" r:id="rId42"/>
+    <hyperlink ref="F5" r:id="rId43" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab6.html"/>
+    <hyperlink ref="F7" r:id="rId44" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab9.html"/>
+    <hyperlink ref="F8" r:id="rId45" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab10.html"/>
+    <hyperlink ref="F13" r:id="rId46" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab15.html"/>
+    <hyperlink ref="F10" r:id="rId47" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab13.html"/>
+    <hyperlink ref="F11" r:id="rId48" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab14.html"/>
+    <hyperlink ref="F14" r:id="rId49" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab16.html"/>
+    <hyperlink ref="F15" r:id="rId50" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab17.html"/>
+    <hyperlink ref="F16" r:id="rId51" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab17.html"/>
+    <hyperlink ref="F17" r:id="rId52" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab17.html"/>
+    <hyperlink ref="F26" r:id="rId53" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab29.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 
@@ -744,7 +870,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -756,7 +882,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
'Robot': most problems are solved
</commit_message>
<xml_diff>
--- a/Curriculum.xlsx
+++ b/Curriculum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="312" windowWidth="23652" windowHeight="9708"/>
+    <workbookView xWindow="240" yWindow="312" windowWidth="22800" windowHeight="9324"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +224,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -241,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -256,6 +262,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -561,7 +568,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -596,17 +603,17 @@
         <v>0</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -614,27 +621,27 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3"/>
@@ -712,7 +719,7 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -723,7 +730,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -734,7 +741,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -743,7 +750,7 @@
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="3" t="s">

</xml_diff>

<commit_message>
Set of tasks 'Robot' completed (100%)
</commit_message>
<xml_diff>
--- a/Curriculum.xlsx
+++ b/Curriculum.xlsx
@@ -568,7 +568,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -610,7 +610,7 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="10" t="s">

</xml_diff>

<commit_message>
4_arithmetics_and_lists, task # 6 (get the list median): done, but badly: O(n^2), but, seemingly, should be O(n)
</commit_message>
<xml_diff>
--- a/Curriculum.xlsx
+++ b/Curriculum.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -568,7 +568,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F19" sqref="F19:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -621,7 +621,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="10" t="s">

</xml_diff>

<commit_message>
4_arithmetics_and_lists, task # 11 ('Skyscrapers') done
</commit_message>
<xml_diff>
--- a/Curriculum.xlsx
+++ b/Curriculum.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -568,7 +568,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:F20"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -624,7 +624,7 @@
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="3"/>

</xml_diff>

<commit_message>
4_arithmetics_and_lists, task # 11 removed
</commit_message>
<xml_diff>
--- a/Curriculum.xlsx
+++ b/Curriculum.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Практика: Черепаха</t>
   </si>
@@ -214,7 +214,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +233,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -247,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -263,6 +269,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -568,7 +575,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -645,9 +652,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -697,7 +702,7 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -741,7 +746,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -856,18 +861,17 @@
     <hyperlink ref="F2" r:id="rId42"/>
     <hyperlink ref="F5" r:id="rId43" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab6.html"/>
     <hyperlink ref="F7" r:id="rId44" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab9.html"/>
-    <hyperlink ref="F8" r:id="rId45" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab10.html"/>
-    <hyperlink ref="F13" r:id="rId46" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab15.html"/>
-    <hyperlink ref="F10" r:id="rId47" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab13.html"/>
-    <hyperlink ref="F11" r:id="rId48" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab14.html"/>
-    <hyperlink ref="F14" r:id="rId49" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab16.html"/>
-    <hyperlink ref="F15" r:id="rId50" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab17.html"/>
-    <hyperlink ref="F16" r:id="rId51" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab17.html"/>
-    <hyperlink ref="F17" r:id="rId52" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab17.html"/>
-    <hyperlink ref="F26" r:id="rId53" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab29.html"/>
+    <hyperlink ref="F13" r:id="rId45" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab15.html"/>
+    <hyperlink ref="F10" r:id="rId46" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab13.html"/>
+    <hyperlink ref="F11" r:id="rId47" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab14.html"/>
+    <hyperlink ref="F14" r:id="rId48" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab16.html"/>
+    <hyperlink ref="F15" r:id="rId49" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab17.html"/>
+    <hyperlink ref="F16" r:id="rId50" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab17.html"/>
+    <hyperlink ref="F17" r:id="rId51" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab17.html"/>
+    <hyperlink ref="F26" r:id="rId52" display="http://judge.mipt.ru/mipt_cs_on_python3_2015/labs/lab29.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId53"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Finish Task 1 (plotting)
</commit_message>
<xml_diff>
--- a/Curriculum.xlsx
+++ b/Curriculum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="312" windowWidth="19128" windowHeight="8952" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="312" windowWidth="19128" windowHeight="8952"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="2" r:id="rId1"/>
@@ -578,7 +578,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +603,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -617,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -668,6 +674,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -972,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,16 +1007,16 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="21" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15">
+      <c r="A3" s="18">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="19" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1034,16 +1049,16 @@
       </c>
     </row>
     <row r="6" spans="1:4" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="25" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1861,7 +1876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>

</xml_diff>